<commit_message>
Update list signals, add links pump control
</commit_message>
<xml_diff>
--- a/Docs/Перечень сигналов.xlsx
+++ b/Docs/Перечень сигналов.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
   <si>
     <t>№</t>
   </si>
@@ -223,12 +223,6 @@
     <t>DO_Light_Heating_Ready</t>
   </si>
   <si>
-    <t>DO_Cmd_HydroPump_Piston_On</t>
-  </si>
-  <si>
-    <t>DO_Cmd_HydroPump_Piston_Off</t>
-  </si>
-  <si>
     <t>DI_Btn_Extruder_Start</t>
   </si>
   <si>
@@ -281,6 +275,108 @@
   </si>
   <si>
     <t>DI_Sn_Extruder_MatOnConv</t>
+  </si>
+  <si>
+    <t>Красный индикатор на панели - Ошибка</t>
+  </si>
+  <si>
+    <t>Индикатор готовности после включения нагрева(45-60 минут)</t>
+  </si>
+  <si>
+    <t>Кнопка включения нагрева</t>
+  </si>
+  <si>
+    <t>Выбор режима работы экструдера - с работой таймера и без него</t>
+  </si>
+  <si>
+    <t>DO_Light_NoMaterial</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>Красный индикатор окончания материала в гидростанции(можно запаралелить с сигналом датчика)</t>
+  </si>
+  <si>
+    <t>DO_BtnLight_Extruder_Work</t>
+  </si>
+  <si>
+    <t>Кнопка включения работы экструдера в автоматическом режиме</t>
+  </si>
+  <si>
+    <t>Индикатор кнопки включения работы экструдера в автоматическом режиме</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>DO_Light_HeatOffWait</t>
+  </si>
+  <si>
+    <t>Индикатор остывания после выключения нагрева(задержка по времени)</t>
+  </si>
+  <si>
+    <t>Выбор направления движения цилиндра в речном режиме</t>
+  </si>
+  <si>
+    <t>Выбор режима работы цилиндра гидронасоса</t>
+  </si>
+  <si>
+    <t>Кнопка включения работы гидронасоса</t>
+  </si>
+  <si>
+    <t>DI_Btn_HydroPump_Stop</t>
+  </si>
+  <si>
+    <t>Кнопка выключения работы гидронасоса</t>
+  </si>
+  <si>
+    <t>Переключатель включения конвейера экструдера</t>
+  </si>
+  <si>
+    <t>DO_Cmd_HydroPump_Piston_Push</t>
+  </si>
+  <si>
+    <t>DO_Cmd_HydroPump_Piston_Pull</t>
+  </si>
+  <si>
+    <t>Команда управления цилиндром гидронасоса на подачу</t>
+  </si>
+  <si>
+    <t>Команда управления цилиндром гидронасоса от насоса</t>
+  </si>
+  <si>
+    <t>Команда включения гидронасоса</t>
+  </si>
+  <si>
+    <t>Команда включения нагрева</t>
+  </si>
+  <si>
+    <t>Нагреватель 1 включен</t>
+  </si>
+  <si>
+    <t>Нагреватель 2 включен</t>
+  </si>
+  <si>
+    <t>Датчик открытия крышки экструдера</t>
+  </si>
+  <si>
+    <t>Датчик окончания материала в гидростанции</t>
+  </si>
+  <si>
+    <t>Команда включения конвееера</t>
+  </si>
+  <si>
+    <t>Команда выдвижения ролика 1</t>
+  </si>
+  <si>
+    <t>Команда выдвижения ролика 2</t>
+  </si>
+  <si>
+    <t>Команда подачи материала на выход экструдера</t>
+  </si>
+  <si>
+    <t>Датчик начала подачи детали на конвейер</t>
   </si>
 </sst>
 </file>
@@ -696,6 +792,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -747,14 +846,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,8 +887,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>589387</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>27700</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19418</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1111,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,32 +1217,32 @@
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="13" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
     <col min="7" max="7" width="78.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
@@ -1156,18 +1252,18 @@
       <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="17"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -1179,12 +1275,14 @@
       <c r="F3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1194,12 +1292,14 @@
       <c r="F4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="30"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1209,12 +1309,14 @@
       <c r="F5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="30"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1224,27 +1326,31 @@
       <c r="F6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="30"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="30"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1254,42 +1360,48 @@
       <c r="F8" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="30"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="10"/>
+      <c r="E9" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="31"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>67</v>
+      <c r="E10" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="32" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="33" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1304,9 +1416,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="30"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1315,9 +1427,9 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="30"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1326,9 +1438,9 @@
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="31"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1337,26 +1449,28 @@
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="33" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="35" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="33"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1366,98 +1480,109 @@
       <c r="F16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="33"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="33"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="33"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="33"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="10"/>
+        <v>72</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="33"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="33"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="30" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="31" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1468,9 +1593,9 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="30"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="31"/>
       <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1479,9 +1604,9 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="30"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="31"/>
       <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1490,8 +1615,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="34"/>
       <c r="D26" s="7" t="s">
         <v>30</v>
@@ -1500,94 +1625,110 @@
       <c r="F26" s="8"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="24">
         <v>2</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="30" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="35"/>
+      <c r="E27" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="30"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="31"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="10"/>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="30"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="31"/>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>42</v>
+      <c r="E29" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="30"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="10"/>
+        <v>38</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="30"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="10"/>
+      <c r="E31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="30"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="30"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1596,9 +1737,9 @@
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="31"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
@@ -1606,90 +1747,114 @@
       <c r="F34" s="4"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="32" t="s">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G35" s="10"/>
+      <c r="E35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="30"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="10"/>
+      <c r="G36" s="10" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="30"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="31"/>
       <c r="D37" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G37" s="10"/>
+        <v>84</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="30"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="31"/>
       <c r="D38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="10"/>
+      <c r="E38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="30"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="31"/>
       <c r="D39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="10"/>
+      <c r="E39" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="30"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="31"/>
       <c r="D40" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="10"/>
+      <c r="E40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="30"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="31"/>
       <c r="D41" s="2" t="s">
         <v>53</v>
       </c>
@@ -1698,8 +1863,8 @@
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="34"/>
       <c r="D42" s="7" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Add manual control pull button
</commit_message>
<xml_diff>
--- a/Docs/Перечень сигналов.xlsx
+++ b/Docs/Перечень сигналов.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="122">
   <si>
     <t>№</t>
   </si>
@@ -217,9 +217,6 @@
     <t>DI_Mode_HydroPump_Auto</t>
   </si>
   <si>
-    <t>DI_Btn_HydroPump_Piston_On</t>
-  </si>
-  <si>
     <t>DO_Light_Heating_Ready</t>
   </si>
   <si>
@@ -377,6 +374,12 @@
   </si>
   <si>
     <t>Датчик начала подачи детали на конвейер</t>
+  </si>
+  <si>
+    <t>DI_Btn_HydroPump_Piston_On_Right</t>
+  </si>
+  <si>
+    <t>DI_Btn_HydroPump_Piston_On_Left</t>
   </si>
 </sst>
 </file>
@@ -795,6 +798,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -815,42 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,7 +1211,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,26 +1226,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
@@ -1252,18 +1255,18 @@
       <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="18"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -1276,13 +1279,13 @@
         <v>40</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1293,13 +1296,13 @@
         <v>41</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1310,13 +1313,13 @@
         <v>39</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1327,30 +1330,30 @@
         <v>56</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="31"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="31"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1361,30 +1364,30 @@
         <v>55</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="31"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>55</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="32"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1395,13 +1398,13 @@
         <v>44</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="33" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="26" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1416,9 +1419,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="31"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1427,9 +1430,9 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="31"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1438,9 +1441,9 @@
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="32"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1449,130 +1452,130 @@
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="35" t="s">
+      <c r="A15" s="18"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="35"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="35"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="35"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="35"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G20" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="35"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="35"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1580,9 +1583,9 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="31" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="24" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1593,9 +1596,9 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="31"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1604,9 +1607,9 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1615,9 +1618,9 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="34"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1625,110 +1628,118 @@
       <c r="F26" s="8"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
         <v>2</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="31"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>105</v>
+      <c r="E28" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="31"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>95</v>
+      <c r="G29" s="16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="31"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>42</v>
+      <c r="E30" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="31"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="10"/>
+      <c r="E32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="31"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1737,9 +1748,9 @@
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="32"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
@@ -1748,113 +1759,113 @@
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="33" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="26" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" t="s">
         <v>91</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="31"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="31"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="31"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="31"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>43</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="31"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="31"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="2" t="s">
         <v>53</v>
       </c>
@@ -1863,9 +1874,9 @@
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="34"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="7" t="s">
         <v>54</v>
       </c>
@@ -1875,6 +1886,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A27:A42"/>
     <mergeCell ref="B27:B42"/>
     <mergeCell ref="C27:C34"/>
@@ -1885,11 +1901,6 @@
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="C15:C22"/>
     <mergeCell ref="C23:C26"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="257" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>